<commit_message>
fix: Correct password hashing logic and update registration number assignment in MembersImport
</commit_message>
<xml_diff>
--- a/public/assets/template-import-anggota.xlsx
+++ b/public/assets/template-import-anggota.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\agro-member-mng\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390D3FA0-6536-436C-9F83-3782D12A6B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDBA292-B9AA-4751-8799-0ED09B74EB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A51EFBB9-38D6-429C-8EF2-FF54273DBB36}"/>
   </bookViews>
@@ -546,8 +546,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E179B6A-7303-4963-9D48-17342C315C80}">
   <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,7 +583,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">

</xml_diff>